<commit_message>
weird errors happening typescript cant view pages in app during this commit
</commit_message>
<xml_diff>
--- a/FileGunBasin/9 August-04 StormBasin/570 new karma or zodiac wizard/pantheonic chepno table 1.xlsx
+++ b/FileGunBasin/9 August-04 StormBasin/570 new karma or zodiac wizard/pantheonic chepno table 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylecampbell/Documents/repos/localrepo-snefuru4/FileGunBasin/9 August-04 StormBasin/570 new karma or zodiac wizard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E28358-E32D-5543-AD5A-30A00C875DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166BB796-49CF-6949-ABBC-839F060A63EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19320" xr2:uid="{50A38606-82DE-8842-84D1-FE3FBCCC812B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>chepno nickel pantheonic</t>
   </si>
@@ -329,6 +329,15 @@
   </si>
   <si>
     <t>in new boulder function</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1iaFhLCfOjc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rAjcXxYTrv4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5PknSpk3m1w</t>
   </si>
 </sst>
 </file>
@@ -829,11 +838,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD632C1F-3CA5-C447-B8E4-947556DA4539}">
-  <dimension ref="A1:H202"/>
+  <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E207" sqref="E207"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E202" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1425,6 +1434,21 @@
         <v>84</v>
       </c>
     </row>
+    <row r="206" spans="4:6">
+      <c r="E206" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="207" spans="4:6">
+      <c r="E207" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="209" spans="5:5">
+      <c r="E209" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E193" r:id="rId1" xr:uid="{FED81138-A76B-1546-AE48-DD69F8F5587E}"/>

</xml_diff>